<commit_message>
use 1017 version benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/201906/jsliu__bank_test_&_city_(HF)(201906)_Loan_Portfolio_Analytics.xlsx
+++ b/lib/report/benchmark_report/web14/exl/201906/jsliu__bank_test_&_city_(HF)(201906)_Loan_Portfolio_Analytics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\THC\R0702\Web ReportTemplates\2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9858685-E519-470D-818A-D263BEADB642}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE045C8-3FA6-444F-851A-28FCB6A17128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortgage Performance" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
     <t>Portfolio Name: Loans and lease financing receivables          Cycle: June, 2019           Evaluation Date: June 28, 2019</t>
   </si>
   <si>
-    <t>Printed on: 08/09/2019 11:05:56AM</t>
+    <t>Printed on: 10/17/2019 2:25:42PM</t>
   </si>
   <si>
     <t>Footnotes:_x000D_
@@ -362,7 +362,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.0000;\-#,##0.0000;\-"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="9"/>
@@ -410,6 +410,13 @@
       <b/>
       <sz val="20"/>
       <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF0E153C"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -820,6 +827,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -847,67 +914,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -987,6 +994,10 @@
       <rgbColor rgb="00333333"/>
       <rgbColor rgb="00999999"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0E153C"/>
+      <color rgb="FF3EBFC8"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1154,7 +1165,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2EA6-4562-9751-311D7B1FD9F4}"/>
+              <c16:uniqueId val="{00000000-7176-4573-8136-977B76714B37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1199,7 +1210,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1300,7 +1311,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8137-40D3-8343-055ED2A8616D}"/>
+              <c16:uniqueId val="{00000000-A065-4889-8423-DD5187830925}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1345,7 +1356,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1530,371 +1541,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="矩形 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="590550"/>
-          <a:ext cx="10086975" cy="10115550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>DISCLAIMER </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>
-            </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>This report and the content contained herein (“Report”) has been generated using the proprietary software and models of Thomas Ho Company Ltd (“THC”) as of the date of this Report. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>This Report contains confidential and/or proprietary information and is intended solely for the benefit of the authorized user of THC’s services. If you are not the intended and authorized user, you should return this Report to THC immediately and in any event shall not disclose, use, copy, or reproduce this Report or its contents, and shall not display or distribute this Report or its contents to any other party without THC’s prior written authorization.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>Nothing in this Report is intended to substitute for any party’s obligations to comply with any applicable laws or regulations. This Report and any information herein may not be relied upon by any other person or entity, including any regulatory authority. Without limiting the foregoing, THC shall not be liable for any losses or damages which may arise directly or indirectly from such reliance, including any incidental, consequential or punitive losses or damages. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>While due care is used in ensuring the content generated in the Report is accurate, the accuracy, completeness and currency of the Report cannot be guaranteed. The THC proprietary software and models may be changed or updated from time to time and future report(s) may be different from current Report, in form or in substance, including such arising from the same data input. THC has no obligation to notify you of any updates or changes of its proprietary software or models, or the existence or content of Report(s) that may be generated using updated or changed software or models. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>THC MAKES NO REPRESENTATION OR WARRANTY, EXPRESS OR IMPLIED, AS TO THE ACCURACY, COMPLETENESS OR CURRENCY OF THE REPORT HEREIN. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> This Report is generated based on data input. It is the responsibility of the person or entity that provided the data input to verify the accuracy and completeness of such data input. THC shall not be responsible to verify the accuracy and completeness of the data input provided by any person or entity other than THC. THC shall not be held liable for any errors or omissions of such data input and shall not be held liable for any direct or indirect losses or damages as the result of or arising out of such errors or omissions, including any incidental, consequential or punitive losses or damages. THC shall not be obligated or liable for any errors or omissions of any third party or events beyond THC’s reasonable control.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>THC is not a registered investment advisor or broker/dealer and does not provide investment advice to any person or entity. Information contained in this Report shall not be construed as any advice or recommendation for trade or investment or otherwise, and is not intended to substitute for obtaining any investment or trade advice. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>THC is not an accounting firm, legal or tax advisor. Information contained in this Report shall not be construed as any accounting, legal or tax advice, and is not intended to substitute for obtaining accounting, legal or tax advice. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>Before acting on any information provided in this Report you should conduct your own due diligence to evaluate the accuracy, completeness and usefulness of the information therein, as well as the risks associated with using THC’s models and related services, and in particular, you should seek independent investment, legal, tax and accounting advice.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>THC’s models embedded in THC’s proprietary software in generating the Report are based on theoretical simulations. The projections or other information generated using THC’s models regarding the likelihood of various balance sheet outcomes or other outcomes are hypothetical in nature. While due care has been used in the operating or running of THC’s models, actual results may vary in a materially positive or negative manner.  Therefore there is no guarantee of future results in using THC’s models. Performance analysis is based on certain assumptions with respect to significant factor(s) that may prove not to be as assumed, such assumptions regarding future events are very difficult if not impossible to predict, and many are beyond THC’s control.  Accordingly, there can be no assurance that the projections, analyses or information this Report generated using THC’s models will prove accurate, complete or consistent. THC shall not be liable for any losses or damages which may arise directly or indirectly from use of or reliance on THC’s models, as well as the information contained in this Report, including any incidental, consequential or punitive losses or damages.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>Without limiting the generality of the foregoing, THIS REPORT IS PROVIDED ‘AS IS’, WITHOUT REPRESENTATIONS OR WARRANTIES OF ANY KIND, EXPRESS OR IMPLIED.  TO THE MAXIMUM EXTENT PERMISSIBLE UNDER APPLICABLE LAW; THC HEREBY DISCLAIMS ANY AND ALL WARRANTIES, EXPRESS AND IMPLIED, RELATING TO THIS REPORT OR ANY INFROMATION CONTAINED HEREIN. THC HEREBY DISCLAIMS, ANY AND ALL WARRANTIES, EXPRESS OR IMPLIED, INCLUDING WARRANTIES OF MECHANTABILITY AND FITNESS FOR A PARTICULAR PURPOSE. THC HEREBY DISCLAIMS, ANY AND ALL REPRESENTATIONS, EXPRESS OR IMPLIED, INCLUDING REPRESENTATIONS CONCERNING THE QUALITY OF THE THC MODELS AND DOES NOT PROMISE THAT THE MODELS WILL PRODUCE ANY ANTICIPATED OR PROJECTED RESULTS, ANALYSES OR INFORMATION, OR BE ERROR FREE. NEITHER THC NOR ANY OF ITS AFFILIATES SHALL IN ANY EVENT BE LIABLE FOR ANY DAMAGES OR LOSSES OF ANY NATURE WHATSOEVER, INCLUDING, BUT NOT LIMITED TO, DIRECT, INDIRECT, INCIDENTAL, CONSEQUENTIAL, EXEMPLARY, SPECIAL AND PUNITIVE DAMAGES, LOSS OF PROFITS OR TRADING LOSSES, RESULTING FROM ANY PERSON’S USE OR RELIANCE UPON, OR INABILITY TO USE, THIS REPORT OR ANY ANALYSES OR INFORMATION CONTAINED HEREIN, EVEN IF THC IS ADVISED OF THE POSSIBILITY OF SUCH DAMAGES OR LOSSES OR IF SUCH DAMAGES OR LOSSES WERE FORESEEABLE.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1945,6 +1591,156 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>742949</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="933450"/>
+          <a:ext cx="10106024" cy="5810251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Disclaimer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>This report and the content contained herein ("Report") has been generated using the proprietary software and models of Thomas Ho Company Ltd ("THC") as of the date of this Report. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>This Report contains confidential and/or proprietary information and is intended solely for the benefit of the authorized user of THC’s services. If you are not the intended and authorized user, you should return this Report to THC immediately and in any event shall not disclose, use, copy, or reproduce this Report or its contents, and shall not display or distribute this Report or its contents to any other party without THC’s prior written authorization. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Nothing in this Report is intended to substitute for any party’s obligations to comply with any applicable laws or regulations. This Report and any information herein may not be relied upon by any other person or entity, including any regulatory authority. Without limiting the foregoing, THC shall not be liable for any losses or damages which may arise directly or indirectly from such reliance, including any incidental, consequential or punitive losses or damages. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>While due care is used in ensuring the content generated in the Report is accurate, the accuracy, completeness and currency of the Report cannot be guaranteed. The THC proprietary software and models may be changed or updated from time to time and future report(s) may be different from current Report, in form or in substance, including such arising from the same data input. THC has no obligation to notify you of any updates or changes of its proprietary software or models, or the existence or content of Report(s) that may be generated using updated or changed software or models. THC MAKES NO REPRESENTATION OR WARRANTY, EXPRESS OR IMPLIED, AS TO THE ACCURACY, COMPLETENESS OR CURRENCY OF THE REPORT HEREIN. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>This Report is generated based on data input. It is the responsibility of the person or entity that provided the data input to verify the accuracy and completeness of such data input. THC shall not be responsible to verify the accuracy and completeness of the data input provided by any person or entity other than THC. THC shall not be held liable for any errors or omissions of such data input and shall not be held liable for any direct or indirect losses or damages as the result of or arising out of such errors or omissions, including any incidental, consequential or punitive losses or damages. THC shall not be obligated or liable for any errors or omissions of any third party or events beyond THC’s reasonable control.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>THC is not a registered investment advisor or broker/dealer and does not provide investment advice to any person or entity. Information contained in this Report shall not be construed as any advice or recommendation for trade or investment or otherwise, and is not intended to substitute for obtaining any investment or trade advice. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>THC is not an accounting firm, legal or tax advisor. Information contained in this Report shall not be construed as any accounting, legal or tax advice, and is not intended to substitute for obtaining accounting, legal or tax advice. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Before acting on any information provided in this Report you should conduct your own due diligence to evaluate the accuracy, completeness and usefulness of the information therein, as well as the risks associated with using THC’s models and related services, and in particular, you should seek independent investment, legal, tax and accounting advice.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050">
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>THC’s models embedded in THC’s proprietary software in generating the Report are based on theoretical simulations. The projections or other information generated using THC’s models regarding the likelihood of various balance sheet outcomes or other outcomes are hypothetical in nature. While due care has been used in the operating or running of THC’s models, actual results may vary in a materially positive or negative manner.  Therefore there is no guarantee of future results in using THC’s models. Performance analysis is based on certain assumptions with respect to significant factor(s) that may prove not to be as assumed, such assumptions regarding future events are very difficult if not impossible to predict, and many are beyond THC’s control.  Accordingly, there can be no assurance that the projections, analyses or information this Report generated using THC’s models will prove accurate, complete or consistent. THC shall not be liable for any losses or damages which may arise directly or indirectly from use of or reliance on THC’s models, as well as the information contained in this Report, including any incidental, consequential or punitive losses or damages. </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2409,29 +2205,29 @@
     <row r="1" spans="2:33" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:33" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:33" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
       <c r="W3" s="33"/>
       <c r="X3" s="33"/>
       <c r="Y3" s="33"/>
@@ -2445,24 +2241,24 @@
       <c r="AG3" s="33"/>
     </row>
     <row r="4" spans="2:33" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
@@ -2481,24 +2277,24 @@
       <c r="AG4" s="24"/>
     </row>
     <row r="5" spans="2:33" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
@@ -2517,24 +2313,24 @@
       <c r="AG5" s="24"/>
     </row>
     <row r="6" spans="2:33" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
       <c r="R6" s="24"/>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
@@ -2553,24 +2349,24 @@
       <c r="AG6" s="24"/>
     </row>
     <row r="7" spans="2:33" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
       <c r="T7" s="25"/>
@@ -2626,10 +2422,10 @@
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="11" t="s">
         <v>8</v>
       </c>
@@ -2639,14 +2435,14 @@
       <c r="G9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -2658,21 +2454,21 @@
       <c r="AG9" s="7"/>
     </row>
     <row r="10" spans="2:33" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="52">
+      <c r="C10" s="43">
         <v>100</v>
       </c>
-      <c r="D10" s="53"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="8">
         <f>C10/100-U17+Q17</f>
         <v>3.4694932269935315</v>
       </c>
       <c r="F10" s="9">
         <f>(1-(C10/10000-U17/100)*AB17)*E17</f>
-        <v>111.40845247436124</v>
+        <v>111.40845247436111</v>
       </c>
       <c r="G10" s="9">
         <f>(1-(C10/10000-U17/100)*AB17)*F17</f>
-        <v>110.85894664600481</v>
+        <v>110.85894664600474</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -2685,173 +2481,173 @@
       <c r="AG10" s="7"/>
     </row>
     <row r="11" spans="2:33" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46" t="s">
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46" t="s">
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46" t="s">
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46" t="s">
+      <c r="X11" s="35"/>
+      <c r="Y11" s="35"/>
+      <c r="Z11" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="AA11" s="46"/>
-      <c r="AB11" s="46"/>
-      <c r="AC11" s="62" t="s">
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="35"/>
+      <c r="AC11" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="AD11" s="63"/>
-      <c r="AE11" s="63"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="44"/>
+      <c r="AD11" s="40"/>
+      <c r="AE11" s="40"/>
+      <c r="AF11" s="40"/>
+      <c r="AG11" s="36"/>
     </row>
     <row r="12" spans="2:33" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="54"/>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="46"/>
+      <c r="C12" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="44" t="s">
+      <c r="I12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="44" t="s">
+      <c r="K12" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="44" t="s">
+      <c r="L12" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="44" t="s">
+      <c r="M12" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="N12" s="44" t="s">
+      <c r="N12" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="44" t="s">
+      <c r="O12" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="P12" s="44" t="s">
+      <c r="P12" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="Q12" s="44" t="s">
+      <c r="Q12" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="R12" s="44" t="s">
+      <c r="R12" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="S12" s="44" t="s">
+      <c r="S12" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="T12" s="44" t="s">
+      <c r="T12" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="U12" s="44" t="s">
+      <c r="U12" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="V12" s="44" t="s">
+      <c r="V12" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="W12" s="44" t="s">
+      <c r="W12" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="X12" s="44" t="s">
+      <c r="X12" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="Y12" s="44" t="s">
+      <c r="Y12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="Z12" s="44" t="s">
+      <c r="Z12" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AA12" s="44" t="s">
+      <c r="AA12" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AB12" s="44" t="s">
+      <c r="AB12" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="AC12" s="46" t="s">
+      <c r="AC12" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="AD12" s="46"/>
-      <c r="AE12" s="46" t="s">
+      <c r="AD12" s="35"/>
+      <c r="AE12" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="AF12" s="46"/>
-      <c r="AG12" s="44" t="s">
+      <c r="AF12" s="35"/>
+      <c r="AG12" s="36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:33" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
-      <c r="Z13" s="44"/>
-      <c r="AA13" s="44"/>
-      <c r="AB13" s="44"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="36"/>
       <c r="AC13" s="32" t="s">
         <v>45</v>
       </c>
@@ -2864,121 +2660,121 @@
       <c r="AF13" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AG13" s="44"/>
+      <c r="AG13" s="36"/>
     </row>
     <row r="14" spans="2:33" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="49" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R14" s="49" t="s">
+      <c r="R14" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="S14" s="49" t="s">
+      <c r="S14" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="T14" s="49" t="s">
+      <c r="T14" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="U14" s="49" t="s">
+      <c r="U14" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="V14" s="49"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="47"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="37"/>
+      <c r="AA14" s="37"/>
+      <c r="AB14" s="37"/>
+      <c r="AC14" s="37"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="37"/>
     </row>
     <row r="15" spans="2:33" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="49"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="48"/>
-      <c r="AA15" s="48"/>
-      <c r="AB15" s="48"/>
-      <c r="AC15" s="48"/>
-      <c r="AD15" s="48"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="48"/>
-      <c r="AG15" s="48"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="38"/>
+      <c r="Y15" s="38"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="38"/>
+      <c r="AB15" s="38"/>
+      <c r="AC15" s="38"/>
+      <c r="AD15" s="38"/>
+      <c r="AE15" s="38"/>
+      <c r="AF15" s="38"/>
+      <c r="AG15" s="38"/>
     </row>
     <row r="16" spans="2:33" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="45"/>
-      <c r="AA16" s="45"/>
-      <c r="AB16" s="45"/>
-      <c r="AC16" s="45"/>
-      <c r="AD16" s="45"/>
-      <c r="AE16" s="45"/>
-      <c r="AF16" s="45"/>
-      <c r="AG16" s="45"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="41"/>
+      <c r="AA16" s="41"/>
+      <c r="AB16" s="41"/>
+      <c r="AC16" s="41"/>
+      <c r="AD16" s="41"/>
+      <c r="AE16" s="41"/>
+      <c r="AF16" s="41"/>
+      <c r="AG16" s="41"/>
     </row>
     <row r="17" spans="1:33" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
@@ -2998,11 +2794,11 @@
       </c>
       <c r="F17" s="13">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!F101:F112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
-        <v>109.58481263349725</v>
+        <v>109.58481263349731</v>
       </c>
       <c r="G17" s="14">
         <f>SUM(DATATEMP!G101:G112)</f>
-        <v>1907.888093315541</v>
+        <v>1907.8880933155419</v>
       </c>
       <c r="H17" s="14">
         <f>SUM(DATATEMP!H101:H112)</f>
@@ -3040,7 +2836,7 @@
       </c>
       <c r="R17" s="17">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!R101:R112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
-        <v>1.8944597237977834</v>
+        <v>1.8944597237977832</v>
       </c>
       <c r="S17" s="17">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!S101:S112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
@@ -3064,15 +2860,15 @@
       </c>
       <c r="X17" s="13">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!X101:X112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
-        <v>2.1330271633782272</v>
+        <v>2.1330271633779834</v>
       </c>
       <c r="Y17" s="13">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!Y101:Y112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
-        <v>7.5191814389567235E-2</v>
+        <v>7.5191814384708761E-2</v>
       </c>
       <c r="Z17" s="18">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!Z101:Z112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
-        <v>3.3948269851725138E-2</v>
+        <v>3.3948269851725117E-2</v>
       </c>
       <c r="AA17" s="13">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!AA101:AA112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
@@ -3080,7 +2876,7 @@
       </c>
       <c r="AB17" s="13">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!AB101:AB112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
-        <v>2.8324379110654356</v>
+        <v>2.8324379110651918</v>
       </c>
       <c r="AC17" s="13">
         <f>IF(SUM(DATATEMP!H101:H112) = 0,"",SUMPRODUCT(DATATEMP!AC101:AC112,DATATEMP!H101:H112)/SUM(DATATEMP!H101:H112))</f>
@@ -3758,10 +3554,10 @@
         <v>114.769478173511</v>
       </c>
       <c r="F30" s="27">
-        <v>114.23495514392602</v>
+        <v>114.2349551439263</v>
       </c>
       <c r="G30" s="28">
-        <v>378.69272100674101</v>
+        <v>378.69272100674198</v>
       </c>
       <c r="H30" s="28">
         <v>331.50336561135902</v>
@@ -3785,10 +3581,10 @@
         <v>75</v>
       </c>
       <c r="Q30" s="30">
-        <v>3.0179728596111439</v>
+        <v>3.0179728596111435</v>
       </c>
       <c r="R30" s="30">
-        <v>1.8352155259661294</v>
+        <v>1.8352155259661289</v>
       </c>
       <c r="S30" s="30">
         <v>-3.9911537650359499E-2</v>
@@ -3800,25 +3596,25 @@
         <v>1.00042165214473</v>
       </c>
       <c r="V30" s="30">
-        <v>1.0861859732241901</v>
+        <v>1.0861859732241903</v>
       </c>
       <c r="W30" s="27">
         <v>2.86794439017438</v>
       </c>
       <c r="X30" s="27">
-        <v>1.3709284378118951</v>
+        <v>1.3709284378106157</v>
       </c>
       <c r="Y30" s="27">
-        <v>-0.60255579590449349</v>
+        <v>-0.60255579593000963</v>
       </c>
       <c r="Z30" s="31">
-        <v>8.1741426922871993E-2</v>
+        <v>8.1741426922871896E-2</v>
       </c>
       <c r="AA30" s="27">
-        <v>0.91352012993625709</v>
+        <v>0.91352012993625697</v>
       </c>
       <c r="AB30" s="27">
-        <v>2.6106362859701555</v>
+        <v>2.610636285968873</v>
       </c>
       <c r="AC30" s="27">
         <v>25.015813009504601</v>
@@ -4925,992 +4721,992 @@
       <c r="AG50" s="28"/>
     </row>
     <row r="51" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
-      <c r="M51" s="36"/>
-      <c r="N51" s="36"/>
-      <c r="O51" s="36"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="36"/>
-      <c r="R51" s="36"/>
-      <c r="S51" s="36"/>
-      <c r="T51" s="36"/>
-      <c r="U51" s="36"/>
-      <c r="V51" s="36"/>
-      <c r="W51" s="36"/>
-      <c r="X51" s="36"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="36"/>
-      <c r="AA51" s="36"/>
-      <c r="AB51" s="36"/>
-      <c r="AC51" s="36"/>
-      <c r="AD51" s="36"/>
-      <c r="AE51" s="36"/>
-      <c r="AF51" s="36"/>
-      <c r="AG51" s="37"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="56"/>
+      <c r="P51" s="56"/>
+      <c r="Q51" s="56"/>
+      <c r="R51" s="56"/>
+      <c r="S51" s="56"/>
+      <c r="T51" s="56"/>
+      <c r="U51" s="56"/>
+      <c r="V51" s="56"/>
+      <c r="W51" s="56"/>
+      <c r="X51" s="56"/>
+      <c r="Y51" s="56"/>
+      <c r="Z51" s="56"/>
+      <c r="AA51" s="56"/>
+      <c r="AB51" s="56"/>
+      <c r="AC51" s="56"/>
+      <c r="AD51" s="56"/>
+      <c r="AE51" s="56"/>
+      <c r="AF51" s="56"/>
+      <c r="AG51" s="57"/>
     </row>
     <row r="52" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="38"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="39"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="39"/>
-      <c r="R52" s="39"/>
-      <c r="S52" s="39"/>
-      <c r="T52" s="39"/>
-      <c r="U52" s="39"/>
-      <c r="V52" s="39"/>
-      <c r="W52" s="39"/>
-      <c r="X52" s="39"/>
-      <c r="Y52" s="39"/>
-      <c r="Z52" s="39"/>
-      <c r="AA52" s="39"/>
-      <c r="AB52" s="39"/>
-      <c r="AC52" s="39"/>
-      <c r="AD52" s="39"/>
-      <c r="AE52" s="39"/>
-      <c r="AF52" s="39"/>
-      <c r="AG52" s="40"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="59"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="59"/>
+      <c r="M52" s="59"/>
+      <c r="N52" s="59"/>
+      <c r="O52" s="59"/>
+      <c r="P52" s="59"/>
+      <c r="Q52" s="59"/>
+      <c r="R52" s="59"/>
+      <c r="S52" s="59"/>
+      <c r="T52" s="59"/>
+      <c r="U52" s="59"/>
+      <c r="V52" s="59"/>
+      <c r="W52" s="59"/>
+      <c r="X52" s="59"/>
+      <c r="Y52" s="59"/>
+      <c r="Z52" s="59"/>
+      <c r="AA52" s="59"/>
+      <c r="AB52" s="59"/>
+      <c r="AC52" s="59"/>
+      <c r="AD52" s="59"/>
+      <c r="AE52" s="59"/>
+      <c r="AF52" s="59"/>
+      <c r="AG52" s="60"/>
     </row>
     <row r="53" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="38"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39"/>
-      <c r="O53" s="39"/>
-      <c r="P53" s="39"/>
-      <c r="Q53" s="39"/>
-      <c r="R53" s="39"/>
-      <c r="S53" s="39"/>
-      <c r="T53" s="39"/>
-      <c r="U53" s="39"/>
-      <c r="V53" s="39"/>
-      <c r="W53" s="39"/>
-      <c r="X53" s="39"/>
-      <c r="Y53" s="39"/>
-      <c r="Z53" s="39"/>
-      <c r="AA53" s="39"/>
-      <c r="AB53" s="39"/>
-      <c r="AC53" s="39"/>
-      <c r="AD53" s="39"/>
-      <c r="AE53" s="39"/>
-      <c r="AF53" s="39"/>
-      <c r="AG53" s="40"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="59"/>
+      <c r="R53" s="59"/>
+      <c r="S53" s="59"/>
+      <c r="T53" s="59"/>
+      <c r="U53" s="59"/>
+      <c r="V53" s="59"/>
+      <c r="W53" s="59"/>
+      <c r="X53" s="59"/>
+      <c r="Y53" s="59"/>
+      <c r="Z53" s="59"/>
+      <c r="AA53" s="59"/>
+      <c r="AB53" s="59"/>
+      <c r="AC53" s="59"/>
+      <c r="AD53" s="59"/>
+      <c r="AE53" s="59"/>
+      <c r="AF53" s="59"/>
+      <c r="AG53" s="60"/>
     </row>
     <row r="54" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="38"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
-      <c r="N54" s="39"/>
-      <c r="O54" s="39"/>
-      <c r="P54" s="39"/>
-      <c r="Q54" s="39"/>
-      <c r="R54" s="39"/>
-      <c r="S54" s="39"/>
-      <c r="T54" s="39"/>
-      <c r="U54" s="39"/>
-      <c r="V54" s="39"/>
-      <c r="W54" s="39"/>
-      <c r="X54" s="39"/>
-      <c r="Y54" s="39"/>
-      <c r="Z54" s="39"/>
-      <c r="AA54" s="39"/>
-      <c r="AB54" s="39"/>
-      <c r="AC54" s="39"/>
-      <c r="AD54" s="39"/>
-      <c r="AE54" s="39"/>
-      <c r="AF54" s="39"/>
-      <c r="AG54" s="40"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59"/>
+      <c r="S54" s="59"/>
+      <c r="T54" s="59"/>
+      <c r="U54" s="59"/>
+      <c r="V54" s="59"/>
+      <c r="W54" s="59"/>
+      <c r="X54" s="59"/>
+      <c r="Y54" s="59"/>
+      <c r="Z54" s="59"/>
+      <c r="AA54" s="59"/>
+      <c r="AB54" s="59"/>
+      <c r="AC54" s="59"/>
+      <c r="AD54" s="59"/>
+      <c r="AE54" s="59"/>
+      <c r="AF54" s="59"/>
+      <c r="AG54" s="60"/>
     </row>
     <row r="55" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="38"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
-      <c r="O55" s="39"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="39"/>
-      <c r="R55" s="39"/>
-      <c r="S55" s="39"/>
-      <c r="T55" s="39"/>
-      <c r="U55" s="39"/>
-      <c r="V55" s="39"/>
-      <c r="W55" s="39"/>
-      <c r="X55" s="39"/>
-      <c r="Y55" s="39"/>
-      <c r="Z55" s="39"/>
-      <c r="AA55" s="39"/>
-      <c r="AB55" s="39"/>
-      <c r="AC55" s="39"/>
-      <c r="AD55" s="39"/>
-      <c r="AE55" s="39"/>
-      <c r="AF55" s="39"/>
-      <c r="AG55" s="40"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="59"/>
+      <c r="R55" s="59"/>
+      <c r="S55" s="59"/>
+      <c r="T55" s="59"/>
+      <c r="U55" s="59"/>
+      <c r="V55" s="59"/>
+      <c r="W55" s="59"/>
+      <c r="X55" s="59"/>
+      <c r="Y55" s="59"/>
+      <c r="Z55" s="59"/>
+      <c r="AA55" s="59"/>
+      <c r="AB55" s="59"/>
+      <c r="AC55" s="59"/>
+      <c r="AD55" s="59"/>
+      <c r="AE55" s="59"/>
+      <c r="AF55" s="59"/>
+      <c r="AG55" s="60"/>
     </row>
     <row r="56" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="38"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="39"/>
-      <c r="N56" s="39"/>
-      <c r="O56" s="39"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="39"/>
-      <c r="R56" s="39"/>
-      <c r="S56" s="39"/>
-      <c r="T56" s="39"/>
-      <c r="U56" s="39"/>
-      <c r="V56" s="39"/>
-      <c r="W56" s="39"/>
-      <c r="X56" s="39"/>
-      <c r="Y56" s="39"/>
-      <c r="Z56" s="39"/>
-      <c r="AA56" s="39"/>
-      <c r="AB56" s="39"/>
-      <c r="AC56" s="39"/>
-      <c r="AD56" s="39"/>
-      <c r="AE56" s="39"/>
-      <c r="AF56" s="39"/>
-      <c r="AG56" s="40"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="59"/>
+      <c r="K56" s="59"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="59"/>
+      <c r="Q56" s="59"/>
+      <c r="R56" s="59"/>
+      <c r="S56" s="59"/>
+      <c r="T56" s="59"/>
+      <c r="U56" s="59"/>
+      <c r="V56" s="59"/>
+      <c r="W56" s="59"/>
+      <c r="X56" s="59"/>
+      <c r="Y56" s="59"/>
+      <c r="Z56" s="59"/>
+      <c r="AA56" s="59"/>
+      <c r="AB56" s="59"/>
+      <c r="AC56" s="59"/>
+      <c r="AD56" s="59"/>
+      <c r="AE56" s="59"/>
+      <c r="AF56" s="59"/>
+      <c r="AG56" s="60"/>
     </row>
     <row r="57" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="38"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="39"/>
-      <c r="N57" s="39"/>
-      <c r="O57" s="39"/>
-      <c r="P57" s="39"/>
-      <c r="Q57" s="39"/>
-      <c r="R57" s="39"/>
-      <c r="S57" s="39"/>
-      <c r="T57" s="39"/>
-      <c r="U57" s="39"/>
-      <c r="V57" s="39"/>
-      <c r="W57" s="39"/>
-      <c r="X57" s="39"/>
-      <c r="Y57" s="39"/>
-      <c r="Z57" s="39"/>
-      <c r="AA57" s="39"/>
-      <c r="AB57" s="39"/>
-      <c r="AC57" s="39"/>
-      <c r="AD57" s="39"/>
-      <c r="AE57" s="39"/>
-      <c r="AF57" s="39"/>
-      <c r="AG57" s="40"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+      <c r="K57" s="59"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="59"/>
+      <c r="N57" s="59"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="59"/>
+      <c r="Q57" s="59"/>
+      <c r="R57" s="59"/>
+      <c r="S57" s="59"/>
+      <c r="T57" s="59"/>
+      <c r="U57" s="59"/>
+      <c r="V57" s="59"/>
+      <c r="W57" s="59"/>
+      <c r="X57" s="59"/>
+      <c r="Y57" s="59"/>
+      <c r="Z57" s="59"/>
+      <c r="AA57" s="59"/>
+      <c r="AB57" s="59"/>
+      <c r="AC57" s="59"/>
+      <c r="AD57" s="59"/>
+      <c r="AE57" s="59"/>
+      <c r="AF57" s="59"/>
+      <c r="AG57" s="60"/>
     </row>
     <row r="58" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="38"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="39"/>
-      <c r="N58" s="39"/>
-      <c r="O58" s="39"/>
-      <c r="P58" s="39"/>
-      <c r="Q58" s="39"/>
-      <c r="R58" s="39"/>
-      <c r="S58" s="39"/>
-      <c r="T58" s="39"/>
-      <c r="U58" s="39"/>
-      <c r="V58" s="39"/>
-      <c r="W58" s="39"/>
-      <c r="X58" s="39"/>
-      <c r="Y58" s="39"/>
-      <c r="Z58" s="39"/>
-      <c r="AA58" s="39"/>
-      <c r="AB58" s="39"/>
-      <c r="AC58" s="39"/>
-      <c r="AD58" s="39"/>
-      <c r="AE58" s="39"/>
-      <c r="AF58" s="39"/>
-      <c r="AG58" s="40"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="59"/>
+      <c r="K58" s="59"/>
+      <c r="L58" s="59"/>
+      <c r="M58" s="59"/>
+      <c r="N58" s="59"/>
+      <c r="O58" s="59"/>
+      <c r="P58" s="59"/>
+      <c r="Q58" s="59"/>
+      <c r="R58" s="59"/>
+      <c r="S58" s="59"/>
+      <c r="T58" s="59"/>
+      <c r="U58" s="59"/>
+      <c r="V58" s="59"/>
+      <c r="W58" s="59"/>
+      <c r="X58" s="59"/>
+      <c r="Y58" s="59"/>
+      <c r="Z58" s="59"/>
+      <c r="AA58" s="59"/>
+      <c r="AB58" s="59"/>
+      <c r="AC58" s="59"/>
+      <c r="AD58" s="59"/>
+      <c r="AE58" s="59"/>
+      <c r="AF58" s="59"/>
+      <c r="AG58" s="60"/>
     </row>
     <row r="59" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="38"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="39"/>
-      <c r="N59" s="39"/>
-      <c r="O59" s="39"/>
-      <c r="P59" s="39"/>
-      <c r="Q59" s="39"/>
-      <c r="R59" s="39"/>
-      <c r="S59" s="39"/>
-      <c r="T59" s="39"/>
-      <c r="U59" s="39"/>
-      <c r="V59" s="39"/>
-      <c r="W59" s="39"/>
-      <c r="X59" s="39"/>
-      <c r="Y59" s="39"/>
-      <c r="Z59" s="39"/>
-      <c r="AA59" s="39"/>
-      <c r="AB59" s="39"/>
-      <c r="AC59" s="39"/>
-      <c r="AD59" s="39"/>
-      <c r="AE59" s="39"/>
-      <c r="AF59" s="39"/>
-      <c r="AG59" s="40"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="59"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="59"/>
+      <c r="R59" s="59"/>
+      <c r="S59" s="59"/>
+      <c r="T59" s="59"/>
+      <c r="U59" s="59"/>
+      <c r="V59" s="59"/>
+      <c r="W59" s="59"/>
+      <c r="X59" s="59"/>
+      <c r="Y59" s="59"/>
+      <c r="Z59" s="59"/>
+      <c r="AA59" s="59"/>
+      <c r="AB59" s="59"/>
+      <c r="AC59" s="59"/>
+      <c r="AD59" s="59"/>
+      <c r="AE59" s="59"/>
+      <c r="AF59" s="59"/>
+      <c r="AG59" s="60"/>
     </row>
     <row r="60" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="38"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39"/>
-      <c r="P60" s="39"/>
-      <c r="Q60" s="39"/>
-      <c r="R60" s="39"/>
-      <c r="S60" s="39"/>
-      <c r="T60" s="39"/>
-      <c r="U60" s="39"/>
-      <c r="V60" s="39"/>
-      <c r="W60" s="39"/>
-      <c r="X60" s="39"/>
-      <c r="Y60" s="39"/>
-      <c r="Z60" s="39"/>
-      <c r="AA60" s="39"/>
-      <c r="AB60" s="39"/>
-      <c r="AC60" s="39"/>
-      <c r="AD60" s="39"/>
-      <c r="AE60" s="39"/>
-      <c r="AF60" s="39"/>
-      <c r="AG60" s="40"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="59"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="59"/>
+      <c r="N60" s="59"/>
+      <c r="O60" s="59"/>
+      <c r="P60" s="59"/>
+      <c r="Q60" s="59"/>
+      <c r="R60" s="59"/>
+      <c r="S60" s="59"/>
+      <c r="T60" s="59"/>
+      <c r="U60" s="59"/>
+      <c r="V60" s="59"/>
+      <c r="W60" s="59"/>
+      <c r="X60" s="59"/>
+      <c r="Y60" s="59"/>
+      <c r="Z60" s="59"/>
+      <c r="AA60" s="59"/>
+      <c r="AB60" s="59"/>
+      <c r="AC60" s="59"/>
+      <c r="AD60" s="59"/>
+      <c r="AE60" s="59"/>
+      <c r="AF60" s="59"/>
+      <c r="AG60" s="60"/>
     </row>
     <row r="61" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="38"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
-      <c r="P61" s="39"/>
-      <c r="Q61" s="39"/>
-      <c r="R61" s="39"/>
-      <c r="S61" s="39"/>
-      <c r="T61" s="39"/>
-      <c r="U61" s="39"/>
-      <c r="V61" s="39"/>
-      <c r="W61" s="39"/>
-      <c r="X61" s="39"/>
-      <c r="Y61" s="39"/>
-      <c r="Z61" s="39"/>
-      <c r="AA61" s="39"/>
-      <c r="AB61" s="39"/>
-      <c r="AC61" s="39"/>
-      <c r="AD61" s="39"/>
-      <c r="AE61" s="39"/>
-      <c r="AF61" s="39"/>
-      <c r="AG61" s="40"/>
+      <c r="B61" s="58"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="59"/>
+      <c r="L61" s="59"/>
+      <c r="M61" s="59"/>
+      <c r="N61" s="59"/>
+      <c r="O61" s="59"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="59"/>
+      <c r="R61" s="59"/>
+      <c r="S61" s="59"/>
+      <c r="T61" s="59"/>
+      <c r="U61" s="59"/>
+      <c r="V61" s="59"/>
+      <c r="W61" s="59"/>
+      <c r="X61" s="59"/>
+      <c r="Y61" s="59"/>
+      <c r="Z61" s="59"/>
+      <c r="AA61" s="59"/>
+      <c r="AB61" s="59"/>
+      <c r="AC61" s="59"/>
+      <c r="AD61" s="59"/>
+      <c r="AE61" s="59"/>
+      <c r="AF61" s="59"/>
+      <c r="AG61" s="60"/>
     </row>
     <row r="62" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="38"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-      <c r="L62" s="39"/>
-      <c r="M62" s="39"/>
-      <c r="N62" s="39"/>
-      <c r="O62" s="39"/>
-      <c r="P62" s="39"/>
-      <c r="Q62" s="39"/>
-      <c r="R62" s="39"/>
-      <c r="S62" s="39"/>
-      <c r="T62" s="39"/>
-      <c r="U62" s="39"/>
-      <c r="V62" s="39"/>
-      <c r="W62" s="39"/>
-      <c r="X62" s="39"/>
-      <c r="Y62" s="39"/>
-      <c r="Z62" s="39"/>
-      <c r="AA62" s="39"/>
-      <c r="AB62" s="39"/>
-      <c r="AC62" s="39"/>
-      <c r="AD62" s="39"/>
-      <c r="AE62" s="39"/>
-      <c r="AF62" s="39"/>
-      <c r="AG62" s="40"/>
+      <c r="B62" s="58"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="59"/>
+      <c r="K62" s="59"/>
+      <c r="L62" s="59"/>
+      <c r="M62" s="59"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="59"/>
+      <c r="P62" s="59"/>
+      <c r="Q62" s="59"/>
+      <c r="R62" s="59"/>
+      <c r="S62" s="59"/>
+      <c r="T62" s="59"/>
+      <c r="U62" s="59"/>
+      <c r="V62" s="59"/>
+      <c r="W62" s="59"/>
+      <c r="X62" s="59"/>
+      <c r="Y62" s="59"/>
+      <c r="Z62" s="59"/>
+      <c r="AA62" s="59"/>
+      <c r="AB62" s="59"/>
+      <c r="AC62" s="59"/>
+      <c r="AD62" s="59"/>
+      <c r="AE62" s="59"/>
+      <c r="AF62" s="59"/>
+      <c r="AG62" s="60"/>
     </row>
     <row r="63" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="38"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
-      <c r="M63" s="39"/>
-      <c r="N63" s="39"/>
-      <c r="O63" s="39"/>
-      <c r="P63" s="39"/>
-      <c r="Q63" s="39"/>
-      <c r="R63" s="39"/>
-      <c r="S63" s="39"/>
-      <c r="T63" s="39"/>
-      <c r="U63" s="39"/>
-      <c r="V63" s="39"/>
-      <c r="W63" s="39"/>
-      <c r="X63" s="39"/>
-      <c r="Y63" s="39"/>
-      <c r="Z63" s="39"/>
-      <c r="AA63" s="39"/>
-      <c r="AB63" s="39"/>
-      <c r="AC63" s="39"/>
-      <c r="AD63" s="39"/>
-      <c r="AE63" s="39"/>
-      <c r="AF63" s="39"/>
-      <c r="AG63" s="40"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="59"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="59"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="59"/>
+      <c r="J63" s="59"/>
+      <c r="K63" s="59"/>
+      <c r="L63" s="59"/>
+      <c r="M63" s="59"/>
+      <c r="N63" s="59"/>
+      <c r="O63" s="59"/>
+      <c r="P63" s="59"/>
+      <c r="Q63" s="59"/>
+      <c r="R63" s="59"/>
+      <c r="S63" s="59"/>
+      <c r="T63" s="59"/>
+      <c r="U63" s="59"/>
+      <c r="V63" s="59"/>
+      <c r="W63" s="59"/>
+      <c r="X63" s="59"/>
+      <c r="Y63" s="59"/>
+      <c r="Z63" s="59"/>
+      <c r="AA63" s="59"/>
+      <c r="AB63" s="59"/>
+      <c r="AC63" s="59"/>
+      <c r="AD63" s="59"/>
+      <c r="AE63" s="59"/>
+      <c r="AF63" s="59"/>
+      <c r="AG63" s="60"/>
     </row>
     <row r="64" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="38"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="39"/>
-      <c r="N64" s="39"/>
-      <c r="O64" s="39"/>
-      <c r="P64" s="39"/>
-      <c r="Q64" s="39"/>
-      <c r="R64" s="39"/>
-      <c r="S64" s="39"/>
-      <c r="T64" s="39"/>
-      <c r="U64" s="39"/>
-      <c r="V64" s="39"/>
-      <c r="W64" s="39"/>
-      <c r="X64" s="39"/>
-      <c r="Y64" s="39"/>
-      <c r="Z64" s="39"/>
-      <c r="AA64" s="39"/>
-      <c r="AB64" s="39"/>
-      <c r="AC64" s="39"/>
-      <c r="AD64" s="39"/>
-      <c r="AE64" s="39"/>
-      <c r="AF64" s="39"/>
-      <c r="AG64" s="40"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="59"/>
+      <c r="F64" s="59"/>
+      <c r="G64" s="59"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="59"/>
+      <c r="J64" s="59"/>
+      <c r="K64" s="59"/>
+      <c r="L64" s="59"/>
+      <c r="M64" s="59"/>
+      <c r="N64" s="59"/>
+      <c r="O64" s="59"/>
+      <c r="P64" s="59"/>
+      <c r="Q64" s="59"/>
+      <c r="R64" s="59"/>
+      <c r="S64" s="59"/>
+      <c r="T64" s="59"/>
+      <c r="U64" s="59"/>
+      <c r="V64" s="59"/>
+      <c r="W64" s="59"/>
+      <c r="X64" s="59"/>
+      <c r="Y64" s="59"/>
+      <c r="Z64" s="59"/>
+      <c r="AA64" s="59"/>
+      <c r="AB64" s="59"/>
+      <c r="AC64" s="59"/>
+      <c r="AD64" s="59"/>
+      <c r="AE64" s="59"/>
+      <c r="AF64" s="59"/>
+      <c r="AG64" s="60"/>
     </row>
     <row r="65" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="38"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="39"/>
-      <c r="N65" s="39"/>
-      <c r="O65" s="39"/>
-      <c r="P65" s="39"/>
-      <c r="Q65" s="39"/>
-      <c r="R65" s="39"/>
-      <c r="S65" s="39"/>
-      <c r="T65" s="39"/>
-      <c r="U65" s="39"/>
-      <c r="V65" s="39"/>
-      <c r="W65" s="39"/>
-      <c r="X65" s="39"/>
-      <c r="Y65" s="39"/>
-      <c r="Z65" s="39"/>
-      <c r="AA65" s="39"/>
-      <c r="AB65" s="39"/>
-      <c r="AC65" s="39"/>
-      <c r="AD65" s="39"/>
-      <c r="AE65" s="39"/>
-      <c r="AF65" s="39"/>
-      <c r="AG65" s="40"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="59"/>
+      <c r="F65" s="59"/>
+      <c r="G65" s="59"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="59"/>
+      <c r="L65" s="59"/>
+      <c r="M65" s="59"/>
+      <c r="N65" s="59"/>
+      <c r="O65" s="59"/>
+      <c r="P65" s="59"/>
+      <c r="Q65" s="59"/>
+      <c r="R65" s="59"/>
+      <c r="S65" s="59"/>
+      <c r="T65" s="59"/>
+      <c r="U65" s="59"/>
+      <c r="V65" s="59"/>
+      <c r="W65" s="59"/>
+      <c r="X65" s="59"/>
+      <c r="Y65" s="59"/>
+      <c r="Z65" s="59"/>
+      <c r="AA65" s="59"/>
+      <c r="AB65" s="59"/>
+      <c r="AC65" s="59"/>
+      <c r="AD65" s="59"/>
+      <c r="AE65" s="59"/>
+      <c r="AF65" s="59"/>
+      <c r="AG65" s="60"/>
     </row>
     <row r="66" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="38"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
-      <c r="M66" s="39"/>
-      <c r="N66" s="39"/>
-      <c r="O66" s="39"/>
-      <c r="P66" s="39"/>
-      <c r="Q66" s="39"/>
-      <c r="R66" s="39"/>
-      <c r="S66" s="39"/>
-      <c r="T66" s="39"/>
-      <c r="U66" s="39"/>
-      <c r="V66" s="39"/>
-      <c r="W66" s="39"/>
-      <c r="X66" s="39"/>
-      <c r="Y66" s="39"/>
-      <c r="Z66" s="39"/>
-      <c r="AA66" s="39"/>
-      <c r="AB66" s="39"/>
-      <c r="AC66" s="39"/>
-      <c r="AD66" s="39"/>
-      <c r="AE66" s="39"/>
-      <c r="AF66" s="39"/>
-      <c r="AG66" s="40"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="59"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="59"/>
+      <c r="J66" s="59"/>
+      <c r="K66" s="59"/>
+      <c r="L66" s="59"/>
+      <c r="M66" s="59"/>
+      <c r="N66" s="59"/>
+      <c r="O66" s="59"/>
+      <c r="P66" s="59"/>
+      <c r="Q66" s="59"/>
+      <c r="R66" s="59"/>
+      <c r="S66" s="59"/>
+      <c r="T66" s="59"/>
+      <c r="U66" s="59"/>
+      <c r="V66" s="59"/>
+      <c r="W66" s="59"/>
+      <c r="X66" s="59"/>
+      <c r="Y66" s="59"/>
+      <c r="Z66" s="59"/>
+      <c r="AA66" s="59"/>
+      <c r="AB66" s="59"/>
+      <c r="AC66" s="59"/>
+      <c r="AD66" s="59"/>
+      <c r="AE66" s="59"/>
+      <c r="AF66" s="59"/>
+      <c r="AG66" s="60"/>
     </row>
     <row r="67" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="38"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-      <c r="L67" s="39"/>
-      <c r="M67" s="39"/>
-      <c r="N67" s="39"/>
-      <c r="O67" s="39"/>
-      <c r="P67" s="39"/>
-      <c r="Q67" s="39"/>
-      <c r="R67" s="39"/>
-      <c r="S67" s="39"/>
-      <c r="T67" s="39"/>
-      <c r="U67" s="39"/>
-      <c r="V67" s="39"/>
-      <c r="W67" s="39"/>
-      <c r="X67" s="39"/>
-      <c r="Y67" s="39"/>
-      <c r="Z67" s="39"/>
-      <c r="AA67" s="39"/>
-      <c r="AB67" s="39"/>
-      <c r="AC67" s="39"/>
-      <c r="AD67" s="39"/>
-      <c r="AE67" s="39"/>
-      <c r="AF67" s="39"/>
-      <c r="AG67" s="40"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="59"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="59"/>
+      <c r="J67" s="59"/>
+      <c r="K67" s="59"/>
+      <c r="L67" s="59"/>
+      <c r="M67" s="59"/>
+      <c r="N67" s="59"/>
+      <c r="O67" s="59"/>
+      <c r="P67" s="59"/>
+      <c r="Q67" s="59"/>
+      <c r="R67" s="59"/>
+      <c r="S67" s="59"/>
+      <c r="T67" s="59"/>
+      <c r="U67" s="59"/>
+      <c r="V67" s="59"/>
+      <c r="W67" s="59"/>
+      <c r="X67" s="59"/>
+      <c r="Y67" s="59"/>
+      <c r="Z67" s="59"/>
+      <c r="AA67" s="59"/>
+      <c r="AB67" s="59"/>
+      <c r="AC67" s="59"/>
+      <c r="AD67" s="59"/>
+      <c r="AE67" s="59"/>
+      <c r="AF67" s="59"/>
+      <c r="AG67" s="60"/>
     </row>
     <row r="68" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="38"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
-      <c r="L68" s="39"/>
-      <c r="M68" s="39"/>
-      <c r="N68" s="39"/>
-      <c r="O68" s="39"/>
-      <c r="P68" s="39"/>
-      <c r="Q68" s="39"/>
-      <c r="R68" s="39"/>
-      <c r="S68" s="39"/>
-      <c r="T68" s="39"/>
-      <c r="U68" s="39"/>
-      <c r="V68" s="39"/>
-      <c r="W68" s="39"/>
-      <c r="X68" s="39"/>
-      <c r="Y68" s="39"/>
-      <c r="Z68" s="39"/>
-      <c r="AA68" s="39"/>
-      <c r="AB68" s="39"/>
-      <c r="AC68" s="39"/>
-      <c r="AD68" s="39"/>
-      <c r="AE68" s="39"/>
-      <c r="AF68" s="39"/>
-      <c r="AG68" s="40"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="59"/>
+      <c r="J68" s="59"/>
+      <c r="K68" s="59"/>
+      <c r="L68" s="59"/>
+      <c r="M68" s="59"/>
+      <c r="N68" s="59"/>
+      <c r="O68" s="59"/>
+      <c r="P68" s="59"/>
+      <c r="Q68" s="59"/>
+      <c r="R68" s="59"/>
+      <c r="S68" s="59"/>
+      <c r="T68" s="59"/>
+      <c r="U68" s="59"/>
+      <c r="V68" s="59"/>
+      <c r="W68" s="59"/>
+      <c r="X68" s="59"/>
+      <c r="Y68" s="59"/>
+      <c r="Z68" s="59"/>
+      <c r="AA68" s="59"/>
+      <c r="AB68" s="59"/>
+      <c r="AC68" s="59"/>
+      <c r="AD68" s="59"/>
+      <c r="AE68" s="59"/>
+      <c r="AF68" s="59"/>
+      <c r="AG68" s="60"/>
     </row>
     <row r="69" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="38"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="39"/>
-      <c r="L69" s="39"/>
-      <c r="M69" s="39"/>
-      <c r="N69" s="39"/>
-      <c r="O69" s="39"/>
-      <c r="P69" s="39"/>
-      <c r="Q69" s="39"/>
-      <c r="R69" s="39"/>
-      <c r="S69" s="39"/>
-      <c r="T69" s="39"/>
-      <c r="U69" s="39"/>
-      <c r="V69" s="39"/>
-      <c r="W69" s="39"/>
-      <c r="X69" s="39"/>
-      <c r="Y69" s="39"/>
-      <c r="Z69" s="39"/>
-      <c r="AA69" s="39"/>
-      <c r="AB69" s="39"/>
-      <c r="AC69" s="39"/>
-      <c r="AD69" s="39"/>
-      <c r="AE69" s="39"/>
-      <c r="AF69" s="39"/>
-      <c r="AG69" s="40"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="59"/>
+      <c r="J69" s="59"/>
+      <c r="K69" s="59"/>
+      <c r="L69" s="59"/>
+      <c r="M69" s="59"/>
+      <c r="N69" s="59"/>
+      <c r="O69" s="59"/>
+      <c r="P69" s="59"/>
+      <c r="Q69" s="59"/>
+      <c r="R69" s="59"/>
+      <c r="S69" s="59"/>
+      <c r="T69" s="59"/>
+      <c r="U69" s="59"/>
+      <c r="V69" s="59"/>
+      <c r="W69" s="59"/>
+      <c r="X69" s="59"/>
+      <c r="Y69" s="59"/>
+      <c r="Z69" s="59"/>
+      <c r="AA69" s="59"/>
+      <c r="AB69" s="59"/>
+      <c r="AC69" s="59"/>
+      <c r="AD69" s="59"/>
+      <c r="AE69" s="59"/>
+      <c r="AF69" s="59"/>
+      <c r="AG69" s="60"/>
     </row>
     <row r="70" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="38"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="39"/>
-      <c r="L70" s="39"/>
-      <c r="M70" s="39"/>
-      <c r="N70" s="39"/>
-      <c r="O70" s="39"/>
-      <c r="P70" s="39"/>
-      <c r="Q70" s="39"/>
-      <c r="R70" s="39"/>
-      <c r="S70" s="39"/>
-      <c r="T70" s="39"/>
-      <c r="U70" s="39"/>
-      <c r="V70" s="39"/>
-      <c r="W70" s="39"/>
-      <c r="X70" s="39"/>
-      <c r="Y70" s="39"/>
-      <c r="Z70" s="39"/>
-      <c r="AA70" s="39"/>
-      <c r="AB70" s="39"/>
-      <c r="AC70" s="39"/>
-      <c r="AD70" s="39"/>
-      <c r="AE70" s="39"/>
-      <c r="AF70" s="39"/>
-      <c r="AG70" s="40"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="59"/>
+      <c r="J70" s="59"/>
+      <c r="K70" s="59"/>
+      <c r="L70" s="59"/>
+      <c r="M70" s="59"/>
+      <c r="N70" s="59"/>
+      <c r="O70" s="59"/>
+      <c r="P70" s="59"/>
+      <c r="Q70" s="59"/>
+      <c r="R70" s="59"/>
+      <c r="S70" s="59"/>
+      <c r="T70" s="59"/>
+      <c r="U70" s="59"/>
+      <c r="V70" s="59"/>
+      <c r="W70" s="59"/>
+      <c r="X70" s="59"/>
+      <c r="Y70" s="59"/>
+      <c r="Z70" s="59"/>
+      <c r="AA70" s="59"/>
+      <c r="AB70" s="59"/>
+      <c r="AC70" s="59"/>
+      <c r="AD70" s="59"/>
+      <c r="AE70" s="59"/>
+      <c r="AF70" s="59"/>
+      <c r="AG70" s="60"/>
     </row>
     <row r="71" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="38"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="39"/>
-      <c r="K71" s="39"/>
-      <c r="L71" s="39"/>
-      <c r="M71" s="39"/>
-      <c r="N71" s="39"/>
-      <c r="O71" s="39"/>
-      <c r="P71" s="39"/>
-      <c r="Q71" s="39"/>
-      <c r="R71" s="39"/>
-      <c r="S71" s="39"/>
-      <c r="T71" s="39"/>
-      <c r="U71" s="39"/>
-      <c r="V71" s="39"/>
-      <c r="W71" s="39"/>
-      <c r="X71" s="39"/>
-      <c r="Y71" s="39"/>
-      <c r="Z71" s="39"/>
-      <c r="AA71" s="39"/>
-      <c r="AB71" s="39"/>
-      <c r="AC71" s="39"/>
-      <c r="AD71" s="39"/>
-      <c r="AE71" s="39"/>
-      <c r="AF71" s="39"/>
-      <c r="AG71" s="40"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="59"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="59"/>
+      <c r="N71" s="59"/>
+      <c r="O71" s="59"/>
+      <c r="P71" s="59"/>
+      <c r="Q71" s="59"/>
+      <c r="R71" s="59"/>
+      <c r="S71" s="59"/>
+      <c r="T71" s="59"/>
+      <c r="U71" s="59"/>
+      <c r="V71" s="59"/>
+      <c r="W71" s="59"/>
+      <c r="X71" s="59"/>
+      <c r="Y71" s="59"/>
+      <c r="Z71" s="59"/>
+      <c r="AA71" s="59"/>
+      <c r="AB71" s="59"/>
+      <c r="AC71" s="59"/>
+      <c r="AD71" s="59"/>
+      <c r="AE71" s="59"/>
+      <c r="AF71" s="59"/>
+      <c r="AG71" s="60"/>
     </row>
     <row r="72" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="38"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="39"/>
-      <c r="L72" s="39"/>
-      <c r="M72" s="39"/>
-      <c r="N72" s="39"/>
-      <c r="O72" s="39"/>
-      <c r="P72" s="39"/>
-      <c r="Q72" s="39"/>
-      <c r="R72" s="39"/>
-      <c r="S72" s="39"/>
-      <c r="T72" s="39"/>
-      <c r="U72" s="39"/>
-      <c r="V72" s="39"/>
-      <c r="W72" s="39"/>
-      <c r="X72" s="39"/>
-      <c r="Y72" s="39"/>
-      <c r="Z72" s="39"/>
-      <c r="AA72" s="39"/>
-      <c r="AB72" s="39"/>
-      <c r="AC72" s="39"/>
-      <c r="AD72" s="39"/>
-      <c r="AE72" s="39"/>
-      <c r="AF72" s="39"/>
-      <c r="AG72" s="40"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
+      <c r="J72" s="59"/>
+      <c r="K72" s="59"/>
+      <c r="L72" s="59"/>
+      <c r="M72" s="59"/>
+      <c r="N72" s="59"/>
+      <c r="O72" s="59"/>
+      <c r="P72" s="59"/>
+      <c r="Q72" s="59"/>
+      <c r="R72" s="59"/>
+      <c r="S72" s="59"/>
+      <c r="T72" s="59"/>
+      <c r="U72" s="59"/>
+      <c r="V72" s="59"/>
+      <c r="W72" s="59"/>
+      <c r="X72" s="59"/>
+      <c r="Y72" s="59"/>
+      <c r="Z72" s="59"/>
+      <c r="AA72" s="59"/>
+      <c r="AB72" s="59"/>
+      <c r="AC72" s="59"/>
+      <c r="AD72" s="59"/>
+      <c r="AE72" s="59"/>
+      <c r="AF72" s="59"/>
+      <c r="AG72" s="60"/>
     </row>
     <row r="73" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="38"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="39"/>
-      <c r="K73" s="39"/>
-      <c r="L73" s="39"/>
-      <c r="M73" s="39"/>
-      <c r="N73" s="39"/>
-      <c r="O73" s="39"/>
-      <c r="P73" s="39"/>
-      <c r="Q73" s="39"/>
-      <c r="R73" s="39"/>
-      <c r="S73" s="39"/>
-      <c r="T73" s="39"/>
-      <c r="U73" s="39"/>
-      <c r="V73" s="39"/>
-      <c r="W73" s="39"/>
-      <c r="X73" s="39"/>
-      <c r="Y73" s="39"/>
-      <c r="Z73" s="39"/>
-      <c r="AA73" s="39"/>
-      <c r="AB73" s="39"/>
-      <c r="AC73" s="39"/>
-      <c r="AD73" s="39"/>
-      <c r="AE73" s="39"/>
-      <c r="AF73" s="39"/>
-      <c r="AG73" s="40"/>
+      <c r="B73" s="58"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
+      <c r="J73" s="59"/>
+      <c r="K73" s="59"/>
+      <c r="L73" s="59"/>
+      <c r="M73" s="59"/>
+      <c r="N73" s="59"/>
+      <c r="O73" s="59"/>
+      <c r="P73" s="59"/>
+      <c r="Q73" s="59"/>
+      <c r="R73" s="59"/>
+      <c r="S73" s="59"/>
+      <c r="T73" s="59"/>
+      <c r="U73" s="59"/>
+      <c r="V73" s="59"/>
+      <c r="W73" s="59"/>
+      <c r="X73" s="59"/>
+      <c r="Y73" s="59"/>
+      <c r="Z73" s="59"/>
+      <c r="AA73" s="59"/>
+      <c r="AB73" s="59"/>
+      <c r="AC73" s="59"/>
+      <c r="AD73" s="59"/>
+      <c r="AE73" s="59"/>
+      <c r="AF73" s="59"/>
+      <c r="AG73" s="60"/>
     </row>
     <row r="74" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="38"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="39"/>
-      <c r="K74" s="39"/>
-      <c r="L74" s="39"/>
-      <c r="M74" s="39"/>
-      <c r="N74" s="39"/>
-      <c r="O74" s="39"/>
-      <c r="P74" s="39"/>
-      <c r="Q74" s="39"/>
-      <c r="R74" s="39"/>
-      <c r="S74" s="39"/>
-      <c r="T74" s="39"/>
-      <c r="U74" s="39"/>
-      <c r="V74" s="39"/>
-      <c r="W74" s="39"/>
-      <c r="X74" s="39"/>
-      <c r="Y74" s="39"/>
-      <c r="Z74" s="39"/>
-      <c r="AA74" s="39"/>
-      <c r="AB74" s="39"/>
-      <c r="AC74" s="39"/>
-      <c r="AD74" s="39"/>
-      <c r="AE74" s="39"/>
-      <c r="AF74" s="39"/>
-      <c r="AG74" s="40"/>
+      <c r="B74" s="58"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="59"/>
+      <c r="K74" s="59"/>
+      <c r="L74" s="59"/>
+      <c r="M74" s="59"/>
+      <c r="N74" s="59"/>
+      <c r="O74" s="59"/>
+      <c r="P74" s="59"/>
+      <c r="Q74" s="59"/>
+      <c r="R74" s="59"/>
+      <c r="S74" s="59"/>
+      <c r="T74" s="59"/>
+      <c r="U74" s="59"/>
+      <c r="V74" s="59"/>
+      <c r="W74" s="59"/>
+      <c r="X74" s="59"/>
+      <c r="Y74" s="59"/>
+      <c r="Z74" s="59"/>
+      <c r="AA74" s="59"/>
+      <c r="AB74" s="59"/>
+      <c r="AC74" s="59"/>
+      <c r="AD74" s="59"/>
+      <c r="AE74" s="59"/>
+      <c r="AF74" s="59"/>
+      <c r="AG74" s="60"/>
     </row>
     <row r="75" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="38"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="39"/>
-      <c r="J75" s="39"/>
-      <c r="K75" s="39"/>
-      <c r="L75" s="39"/>
-      <c r="M75" s="39"/>
-      <c r="N75" s="39"/>
-      <c r="O75" s="39"/>
-      <c r="P75" s="39"/>
-      <c r="Q75" s="39"/>
-      <c r="R75" s="39"/>
-      <c r="S75" s="39"/>
-      <c r="T75" s="39"/>
-      <c r="U75" s="39"/>
-      <c r="V75" s="39"/>
-      <c r="W75" s="39"/>
-      <c r="X75" s="39"/>
-      <c r="Y75" s="39"/>
-      <c r="Z75" s="39"/>
-      <c r="AA75" s="39"/>
-      <c r="AB75" s="39"/>
-      <c r="AC75" s="39"/>
-      <c r="AD75" s="39"/>
-      <c r="AE75" s="39"/>
-      <c r="AF75" s="39"/>
-      <c r="AG75" s="40"/>
+      <c r="B75" s="58"/>
+      <c r="C75" s="59"/>
+      <c r="D75" s="59"/>
+      <c r="E75" s="59"/>
+      <c r="F75" s="59"/>
+      <c r="G75" s="59"/>
+      <c r="H75" s="59"/>
+      <c r="I75" s="59"/>
+      <c r="J75" s="59"/>
+      <c r="K75" s="59"/>
+      <c r="L75" s="59"/>
+      <c r="M75" s="59"/>
+      <c r="N75" s="59"/>
+      <c r="O75" s="59"/>
+      <c r="P75" s="59"/>
+      <c r="Q75" s="59"/>
+      <c r="R75" s="59"/>
+      <c r="S75" s="59"/>
+      <c r="T75" s="59"/>
+      <c r="U75" s="59"/>
+      <c r="V75" s="59"/>
+      <c r="W75" s="59"/>
+      <c r="X75" s="59"/>
+      <c r="Y75" s="59"/>
+      <c r="Z75" s="59"/>
+      <c r="AA75" s="59"/>
+      <c r="AB75" s="59"/>
+      <c r="AC75" s="59"/>
+      <c r="AD75" s="59"/>
+      <c r="AE75" s="59"/>
+      <c r="AF75" s="59"/>
+      <c r="AG75" s="60"/>
     </row>
     <row r="76" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="38"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
-      <c r="F76" s="39"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="39"/>
-      <c r="I76" s="39"/>
-      <c r="J76" s="39"/>
-      <c r="K76" s="39"/>
-      <c r="L76" s="39"/>
-      <c r="M76" s="39"/>
-      <c r="N76" s="39"/>
-      <c r="O76" s="39"/>
-      <c r="P76" s="39"/>
-      <c r="Q76" s="39"/>
-      <c r="R76" s="39"/>
-      <c r="S76" s="39"/>
-      <c r="T76" s="39"/>
-      <c r="U76" s="39"/>
-      <c r="V76" s="39"/>
-      <c r="W76" s="39"/>
-      <c r="X76" s="39"/>
-      <c r="Y76" s="39"/>
-      <c r="Z76" s="39"/>
-      <c r="AA76" s="39"/>
-      <c r="AB76" s="39"/>
-      <c r="AC76" s="39"/>
-      <c r="AD76" s="39"/>
-      <c r="AE76" s="39"/>
-      <c r="AF76" s="39"/>
-      <c r="AG76" s="40"/>
+      <c r="B76" s="58"/>
+      <c r="C76" s="59"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="59"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="59"/>
+      <c r="J76" s="59"/>
+      <c r="K76" s="59"/>
+      <c r="L76" s="59"/>
+      <c r="M76" s="59"/>
+      <c r="N76" s="59"/>
+      <c r="O76" s="59"/>
+      <c r="P76" s="59"/>
+      <c r="Q76" s="59"/>
+      <c r="R76" s="59"/>
+      <c r="S76" s="59"/>
+      <c r="T76" s="59"/>
+      <c r="U76" s="59"/>
+      <c r="V76" s="59"/>
+      <c r="W76" s="59"/>
+      <c r="X76" s="59"/>
+      <c r="Y76" s="59"/>
+      <c r="Z76" s="59"/>
+      <c r="AA76" s="59"/>
+      <c r="AB76" s="59"/>
+      <c r="AC76" s="59"/>
+      <c r="AD76" s="59"/>
+      <c r="AE76" s="59"/>
+      <c r="AF76" s="59"/>
+      <c r="AG76" s="60"/>
     </row>
     <row r="77" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="38"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="39"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="39"/>
-      <c r="I77" s="39"/>
-      <c r="J77" s="39"/>
-      <c r="K77" s="39"/>
-      <c r="L77" s="39"/>
-      <c r="M77" s="39"/>
-      <c r="N77" s="39"/>
-      <c r="O77" s="39"/>
-      <c r="P77" s="39"/>
-      <c r="Q77" s="39"/>
-      <c r="R77" s="39"/>
-      <c r="S77" s="39"/>
-      <c r="T77" s="39"/>
-      <c r="U77" s="39"/>
-      <c r="V77" s="39"/>
-      <c r="W77" s="39"/>
-      <c r="X77" s="39"/>
-      <c r="Y77" s="39"/>
-      <c r="Z77" s="39"/>
-      <c r="AA77" s="39"/>
-      <c r="AB77" s="39"/>
-      <c r="AC77" s="39"/>
-      <c r="AD77" s="39"/>
-      <c r="AE77" s="39"/>
-      <c r="AF77" s="39"/>
-      <c r="AG77" s="40"/>
+      <c r="B77" s="58"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="59"/>
+      <c r="F77" s="59"/>
+      <c r="G77" s="59"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="59"/>
+      <c r="J77" s="59"/>
+      <c r="K77" s="59"/>
+      <c r="L77" s="59"/>
+      <c r="M77" s="59"/>
+      <c r="N77" s="59"/>
+      <c r="O77" s="59"/>
+      <c r="P77" s="59"/>
+      <c r="Q77" s="59"/>
+      <c r="R77" s="59"/>
+      <c r="S77" s="59"/>
+      <c r="T77" s="59"/>
+      <c r="U77" s="59"/>
+      <c r="V77" s="59"/>
+      <c r="W77" s="59"/>
+      <c r="X77" s="59"/>
+      <c r="Y77" s="59"/>
+      <c r="Z77" s="59"/>
+      <c r="AA77" s="59"/>
+      <c r="AB77" s="59"/>
+      <c r="AC77" s="59"/>
+      <c r="AD77" s="59"/>
+      <c r="AE77" s="59"/>
+      <c r="AF77" s="59"/>
+      <c r="AG77" s="60"/>
     </row>
     <row r="78" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="38"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="39"/>
-      <c r="I78" s="39"/>
-      <c r="J78" s="39"/>
-      <c r="K78" s="39"/>
-      <c r="L78" s="39"/>
-      <c r="M78" s="39"/>
-      <c r="N78" s="39"/>
-      <c r="O78" s="39"/>
-      <c r="P78" s="39"/>
-      <c r="Q78" s="39"/>
-      <c r="R78" s="39"/>
-      <c r="S78" s="39"/>
-      <c r="T78" s="39"/>
-      <c r="U78" s="39"/>
-      <c r="V78" s="39"/>
-      <c r="W78" s="39"/>
-      <c r="X78" s="39"/>
-      <c r="Y78" s="39"/>
-      <c r="Z78" s="39"/>
-      <c r="AA78" s="39"/>
-      <c r="AB78" s="39"/>
-      <c r="AC78" s="39"/>
-      <c r="AD78" s="39"/>
-      <c r="AE78" s="39"/>
-      <c r="AF78" s="39"/>
-      <c r="AG78" s="40"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="59"/>
+      <c r="K78" s="59"/>
+      <c r="L78" s="59"/>
+      <c r="M78" s="59"/>
+      <c r="N78" s="59"/>
+      <c r="O78" s="59"/>
+      <c r="P78" s="59"/>
+      <c r="Q78" s="59"/>
+      <c r="R78" s="59"/>
+      <c r="S78" s="59"/>
+      <c r="T78" s="59"/>
+      <c r="U78" s="59"/>
+      <c r="V78" s="59"/>
+      <c r="W78" s="59"/>
+      <c r="X78" s="59"/>
+      <c r="Y78" s="59"/>
+      <c r="Z78" s="59"/>
+      <c r="AA78" s="59"/>
+      <c r="AB78" s="59"/>
+      <c r="AC78" s="59"/>
+      <c r="AD78" s="59"/>
+      <c r="AE78" s="59"/>
+      <c r="AF78" s="59"/>
+      <c r="AG78" s="60"/>
     </row>
     <row r="79" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="41"/>
-      <c r="C79" s="42"/>
-      <c r="D79" s="42"/>
-      <c r="E79" s="42"/>
-      <c r="F79" s="42"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="42"/>
-      <c r="I79" s="42"/>
-      <c r="J79" s="42"/>
-      <c r="K79" s="42"/>
-      <c r="L79" s="42"/>
-      <c r="M79" s="42"/>
-      <c r="N79" s="42"/>
-      <c r="O79" s="42"/>
-      <c r="P79" s="42"/>
-      <c r="Q79" s="42"/>
-      <c r="R79" s="42"/>
-      <c r="S79" s="42"/>
-      <c r="T79" s="42"/>
-      <c r="U79" s="42"/>
-      <c r="V79" s="42"/>
-      <c r="W79" s="42"/>
-      <c r="X79" s="42"/>
-      <c r="Y79" s="42"/>
-      <c r="Z79" s="42"/>
-      <c r="AA79" s="42"/>
-      <c r="AB79" s="42"/>
-      <c r="AC79" s="42"/>
-      <c r="AD79" s="42"/>
-      <c r="AE79" s="42"/>
-      <c r="AF79" s="42"/>
-      <c r="AG79" s="43"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="62"/>
+      <c r="D79" s="62"/>
+      <c r="E79" s="62"/>
+      <c r="F79" s="62"/>
+      <c r="G79" s="62"/>
+      <c r="H79" s="62"/>
+      <c r="I79" s="62"/>
+      <c r="J79" s="62"/>
+      <c r="K79" s="62"/>
+      <c r="L79" s="62"/>
+      <c r="M79" s="62"/>
+      <c r="N79" s="62"/>
+      <c r="O79" s="62"/>
+      <c r="P79" s="62"/>
+      <c r="Q79" s="62"/>
+      <c r="R79" s="62"/>
+      <c r="S79" s="62"/>
+      <c r="T79" s="62"/>
+      <c r="U79" s="62"/>
+      <c r="V79" s="62"/>
+      <c r="W79" s="62"/>
+      <c r="X79" s="62"/>
+      <c r="Y79" s="62"/>
+      <c r="Z79" s="62"/>
+      <c r="AA79" s="62"/>
+      <c r="AB79" s="62"/>
+      <c r="AC79" s="62"/>
+      <c r="AD79" s="62"/>
+      <c r="AE79" s="62"/>
+      <c r="AF79" s="62"/>
+      <c r="AG79" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="65">
@@ -5923,22 +5719,30 @@
     <mergeCell ref="B26:AG26"/>
     <mergeCell ref="B29:AG29"/>
     <mergeCell ref="B33:AG33"/>
-    <mergeCell ref="AC14:AG15"/>
-    <mergeCell ref="AC11:AG11"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AB12:AB13"/>
-    <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="T14:T15"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="Z14:AB15"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="S14:S15"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="W12:W13"/>
-    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="B51:AG79"/>
+    <mergeCell ref="Y12:Y13"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="AA12:AA13"/>
+    <mergeCell ref="B16:AG16"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="W14:Y15"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="E12:E13"/>
@@ -5955,30 +5759,22 @@
     <mergeCell ref="H9:M9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B51:AG79"/>
-    <mergeCell ref="Y12:Y13"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="AA12:AA13"/>
-    <mergeCell ref="B16:AG16"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="S12:S13"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="W14:Y15"/>
-    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AB12:AB13"/>
+    <mergeCell ref="AG12:AG13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="Z14:AB15"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="W12:W13"/>
+    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="AC14:AG15"/>
+    <mergeCell ref="AC11:AG11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.19097222222222221" right="0.19097222222222221" top="0.19097222222222221" bottom="0.19097222222222221" header="0" footer="0"/>
@@ -6002,7 +5798,9 @@
   </sheetPr>
   <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7180,11 +6978,11 @@
       </c>
       <c r="F105">
         <f>'Mortgage Performance'!F30</f>
-        <v>114.23495514392602</v>
+        <v>114.2349551439263</v>
       </c>
       <c r="G105">
         <f>'Mortgage Performance'!G30</f>
-        <v>378.69272100674101</v>
+        <v>378.69272100674198</v>
       </c>
       <c r="H105">
         <f>'Mortgage Performance'!H30</f>
@@ -7224,11 +7022,11 @@
       </c>
       <c r="Q105">
         <f>'Mortgage Performance'!Q30</f>
-        <v>3.0179728596111439</v>
+        <v>3.0179728596111435</v>
       </c>
       <c r="R105">
         <f>'Mortgage Performance'!R30</f>
-        <v>1.8352155259661294</v>
+        <v>1.8352155259661289</v>
       </c>
       <c r="S105">
         <f>'Mortgage Performance'!S30</f>
@@ -7244,7 +7042,7 @@
       </c>
       <c r="V105">
         <f>'Mortgage Performance'!V30</f>
-        <v>1.0861859732241901</v>
+        <v>1.0861859732241903</v>
       </c>
       <c r="W105">
         <f>'Mortgage Performance'!W30</f>
@@ -7252,23 +7050,23 @@
       </c>
       <c r="X105">
         <f>'Mortgage Performance'!X30</f>
-        <v>1.3709284378118951</v>
+        <v>1.3709284378106157</v>
       </c>
       <c r="Y105">
         <f>'Mortgage Performance'!Y30</f>
-        <v>-0.60255579590449349</v>
+        <v>-0.60255579593000963</v>
       </c>
       <c r="Z105">
         <f>'Mortgage Performance'!Z30</f>
-        <v>8.1741426922871993E-2</v>
+        <v>8.1741426922871896E-2</v>
       </c>
       <c r="AA105">
         <f>'Mortgage Performance'!AA30</f>
-        <v>0.91352012993625709</v>
+        <v>0.91352012993625697</v>
       </c>
       <c r="AB105">
         <f>'Mortgage Performance'!AB30</f>
-        <v>2.6106362859701555</v>
+        <v>2.610636285968873</v>
       </c>
       <c r="AC105">
         <f>'Mortgage Performance'!AC30</f>

</xml_diff>